<commit_message>
change form xampp to mamp
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Book_store\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\Book_store\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2717DCA9-5BBF-4CCA-B585-C19307776E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD703F6-B62E-430E-8EB1-4FACA327BB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1080" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A2E77B58-F548-447D-A7DB-A397B28DEA97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A2E77B58-F548-447D-A7DB-A397B28DEA97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>สมาชิก</t>
   </si>
@@ -272,6 +272,9 @@
   <si>
     <t>ทำinsert</t>
   </si>
+  <si>
+    <t>ทานตะวัน</t>
+  </si>
 </sst>
 </file>
 
@@ -450,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -481,19 +484,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -514,20 +526,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,14 +613,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>CREATE TABLE </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US">
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
-            <a:t>user_account</a:t>
-          </a:r>
+            <a:t>CREATE TABLE user_account(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -625,7 +627,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>(</a:t>
+            <a:t>    Username VARCHAR(100) NOT NULL,</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -639,12 +641,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Username</a:t>
-          </a:r>
+            <a:t>    Userpassword VARCHAR(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -655,7 +655,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> VARCHAR(100) NOT NULL PRIMARY KEY,</a:t>
+            <a:t>    first_name VARCHAR(200) NOT NULL,</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -669,12 +669,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Userpassword </a:t>
-          </a:r>
+            <a:t>    last_name VARCHAR(200) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -685,7 +683,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> VARCHAR(100) NOT NULL,</a:t>
+            <a:t>    house_number VARCHAR(60) NOT NULL,</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -699,12 +697,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>first_name</a:t>
-          </a:r>
+            <a:t>    road VARCHAR(60),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -715,7 +711,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> VARCHAR(200) NOT NULL,</a:t>
+            <a:t>    sub_district VARCHAR(255),</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -729,12 +725,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>last_name </a:t>
-          </a:r>
+            <a:t>    district VARCHAR(255) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -745,7 +739,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>VARCHAR(200) NOT NULL,</a:t>
+            <a:t>    provinces VARCHAR(255) NOT NULL,</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -759,12 +753,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>house_number </a:t>
-          </a:r>
+            <a:t>    postal_code VARCHAR(5) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -775,7 +767,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>VARCHAR(60) NOT NULL,</a:t>
+            <a:t>    email VARCHAR(255) NOT NULL,</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -789,12 +781,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>road</a:t>
-          </a:r>
+            <a:t>    PRIMARY KEY(Username)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -805,184 +795,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> VARCHAR(60),</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>sub_district </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>VARCHAR(255),</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>district </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>VARCHAR(255) NOT NULL,</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    provinces VARCHAR(255) NOT NULL,</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>    postal_code varchar(5) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>NOT NULL</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>,</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>email </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>VARCHAR(255) NOT NULL</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
             <a:t>) ENGINE = INNODB DEFAULT CHARSET = utf8;</a:t>
           </a:r>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -2718,6 +2532,1703 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B708481-DFCA-1384-4A15-557F243AD45D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12877800" y="123825"/>
+          <a:ext cx="4067175" cy="4648200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO `user_account`(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `Username`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `Userpassword`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `first_name`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `last_name`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `house_number`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `road`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `sub_district`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `district`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `provinces`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `postal_code`,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    `email`</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES('imonthx','imonthx','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100"/>
+            <a:t>มณกานต์','มีดี','8/8',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>NULL,'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100"/>
+            <a:t>เฟื้องฟ้า','เฟื้องฟ้า','สุพรรณบุรี','11001','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>imonthx@gmail.com'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>('jopper','jopper','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100"/>
+            <a:t>ชนกานต์','ขยันมาก','9/9',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>NULL,'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100"/>
+            <a:t>กุหลาบ','กุหลาบ','สุรินทร์','12345','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>jopper@gmail.com'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>('dewdiw','dewdiw','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100"/>
+            <a:t>สิรวิชญ์','เลิกตื่นสาย','7/7',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>NULL,'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100"/>
+            <a:t>ทานตะวัน','ทานตะวัน','นครราชศ','52345','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>dewdiw@gmail.com')</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5133975" cy="2228850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7329BBB4-2495-068C-8AD3-B8EE48DDA453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12906375" y="3562350"/>
+          <a:ext cx="5133975" cy="2228850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{166AC38A-D558-9DC4-E614-E3C24748D7CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16897349" y="3400424"/>
+          <a:ext cx="4543425" cy="9925051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CREATE TABLE user_account(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    Username VARCHAR(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    Userpassword VARCHAR(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    first_name VARCHAR(200) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    last_name VARCHAR(200) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    house_number VARCHAR(60) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    road VARCHAR(60),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    sub_district VARCHAR(255),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    district VARCHAR(255) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    provinces VARCHAR(255) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    postal_code VARCHAR(5) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    email VARCHAR(255) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    PRIMARY KEY(Username)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>) ENGINE = INNODB DEFAULT CHARSET = utf8;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CREATE TABLE type_book(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    id_typeB CHAR(10) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    typeN VARCHAR(100) NOT NULL UNIQUE,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    PRIMARY KEY(id_typeB)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>) ENGINE = INNODB DEFAULT CHARSET = utf8;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CREATE TABLE publisher_name(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    id_publisher CHAR(10) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    publisherN VARCHAR(100) NOT NULL UNIQUE,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    PRIMARY KEY(id_publisher)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>) ENGINE = INNODB DEFAULT CHARSET = utf8;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CREATE TABLE author(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    id_author CHAR(10) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    authorFN VARCHAR(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    authorLN VARCHAR(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    PRIMARY KEY(id_author)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>) ENGINE = INNODB DEFAULT CHARSET = utf8;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CREATE TABLE book(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    id_isbn CHAR(20) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    id_typeB VARCHAR(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    bookN VARCHAR(200) NOT NULL UNIQUE,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    imgeB VARCHAR(200) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    id_publisher VARCHAR(100),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    id_author VARCHAR(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    price INT(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    amount INT(100) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    PRIMARY KEY(id_isbn),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    FOREIGN KEY(id_typeB) REFERENCES type_book(id_typeB),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    FOREIGN KEY(id_publisher) REFERENCES publisher_name(id_publisher),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>    FOREIGN KEY(id_author) REFERENCES author(id_author)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>) ENGINE = INNODB DEFAULT CHARSET = utf8;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>INSERT INTO `user_account`(`Username`, `Userpassword`, `first_name`, `last_name`, `house_number`, `road`, `sub_district`, `district`, `province`, `postal_code`, `email`) VALUES ('admin','1234','ad','min','12',null,null,'เมือง','สุรินทร์','32000','book.job2012@gmail.com')</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7258050" cy="3638550"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27A5C5A4-6CF8-715F-005A-E216F4F89A3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12973050" y="13458825"/>
+          <a:ext cx="7258050" cy="3638550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="Text Box 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99873150-F787-DA62-E0AA-4B689A7DE739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3724275" y="13039724"/>
+          <a:ext cx="4476750" cy="3438525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>INSERT INTO `author`(`id_author`, `authorFN`, `authorLN`) </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>VALUES </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('A001','Danchun','Zhainan'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('A002','Pingfan','Moshushi'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('C001','สมขยัน','ขยัน'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('D001','ปลา','ตายาว'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('C002','กอไก่','บินได้')</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>INSERT INTO `publisher_name`(`id_publisher`, `publisherN`) </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>VALUES </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('P001','EA'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('G001','Steam'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('G002','Unity'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('E001','Epic'),</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>('T001','Xbox')</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>INSERT INTO `type_book`(`id_typeB`, `typeN`) VALUES ('000','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ทั่วไป(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>General)'),('001','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>การ์ตูน(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Comic)'),('002','</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>นิยาย(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Novel)')</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7648491-6600-5EC4-76D8-D17537E3699D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10039350" y="14116050"/>
+          <a:ext cx="7305675" cy="4886325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>CREATE TABLE image_icon (</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>  id_image INT NOT NULL AUTO_INCREMENT,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>  image_name VARCHAR(200) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>  PRIMARY KEY (id_image)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>) ENGINE=InnoDB DEFAULT CHARSET=utf8;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>CREATE TABLE </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>image_food</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  id_image INT NOT NULL AUTO_INCREMENT,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  image_name VARCHAR(200) NOT NULL,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  PRIMARY KEY (id_image)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>) ENGINE=InnoDB DEFAULT CHARSET=utf8;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11638,7 +13149,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11666,26 +13177,26 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="20"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
@@ -11716,26 +13227,26 @@
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="18"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="4" t="s">
         <v>34</v>
       </c>
@@ -11764,16 +13275,16 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="8"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -11790,16 +13301,16 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="8"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -11816,16 +13327,16 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="8"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -11842,16 +13353,16 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="8"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -11868,16 +13379,16 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="8"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -11894,16 +13405,16 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="8"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -11953,435 +13464,435 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
       <c r="X10" s="5"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19" t="s">
+      <c r="E11" s="32"/>
+      <c r="F11" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="5"/>
       <c r="I11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="19"/>
+      <c r="K11" s="32"/>
       <c r="L11" s="15" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="20" t="s">
+      <c r="O11" s="32"/>
+      <c r="P11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19" t="s">
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19" t="s">
+      <c r="S11" s="32"/>
+      <c r="T11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="U11" s="19"/>
-      <c r="V11" s="20" t="s">
+      <c r="U11" s="32"/>
+      <c r="V11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="W11" s="19"/>
+      <c r="W11" s="32"/>
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="18" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="5"/>
       <c r="I12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="18"/>
+      <c r="K12" s="21"/>
       <c r="L12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="N12" s="18" t="s">
+      <c r="N12" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="22" t="s">
+      <c r="O12" s="21"/>
+      <c r="P12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18" t="s">
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18" t="s">
+      <c r="S12" s="21"/>
+      <c r="T12" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="22" t="s">
+      <c r="U12" s="21"/>
+      <c r="V12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="W12" s="18"/>
+      <c r="W12" s="21"/>
       <c r="X12" s="5"/>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="22"/>
-      <c r="W13" s="18"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="21"/>
       <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="18"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="21"/>
       <c r="X14" s="5"/>
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="5"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="18"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="21"/>
       <c r="X15" s="5"/>
     </row>
     <row r="16" spans="1:24">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="22"/>
-      <c r="W16" s="18"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="21"/>
       <c r="X16" s="5"/>
     </row>
     <row r="17" spans="1:24">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="5"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="18"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="21"/>
       <c r="X17" s="5"/>
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
       <c r="H18" s="5"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="18"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="21"/>
       <c r="X18" s="5"/>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
       <c r="H19" s="5"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="18"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="21"/>
       <c r="X19" s="5"/>
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="18"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="21"/>
       <c r="X20" s="5"/>
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="22"/>
-      <c r="W21" s="18"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="21"/>
       <c r="X21" s="5"/>
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
       <c r="H22" s="5"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="18"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="21"/>
       <c r="X22" s="5"/>
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
       <c r="H23" s="5"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="22"/>
-      <c r="W23" s="18"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="21"/>
       <c r="X23" s="5"/>
     </row>
     <row r="24" spans="1:24">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="18"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="21"/>
       <c r="X24" s="5"/>
     </row>
     <row r="25" spans="1:24">
@@ -12394,20 +13905,20 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="22"/>
-      <c r="W25" s="18"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="21"/>
       <c r="X25" s="5"/>
     </row>
     <row r="26" spans="1:24">
@@ -12463,32 +13974,32 @@
       <c r="X27" s="5"/>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19" t="s">
+      <c r="E28" s="32"/>
+      <c r="F28" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="32"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18" t="s">
+      <c r="J28" s="21"/>
+      <c r="K28" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18" t="s">
+      <c r="L28" s="21"/>
+      <c r="M28" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="N28" s="18"/>
+      <c r="N28" s="21"/>
       <c r="O28" s="5"/>
       <c r="P28" s="4" t="s">
         <v>27</v>
@@ -12496,45 +14007,45 @@
       <c r="Q28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R28" s="18" t="s">
+      <c r="R28" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18" t="s">
+      <c r="S28" s="21"/>
+      <c r="T28" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="U28" s="18"/>
+      <c r="U28" s="21"/>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="19" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19" t="s">
+      <c r="E29" s="32"/>
+      <c r="F29" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="19"/>
+      <c r="G29" s="32"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="27" t="s">
+      <c r="I29" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="J29" s="28"/>
-      <c r="K29" s="18" t="s">
+      <c r="J29" s="31"/>
+      <c r="K29" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18" t="s">
+      <c r="L29" s="21"/>
+      <c r="M29" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N29" s="18"/>
+      <c r="N29" s="21"/>
       <c r="O29" s="5"/>
       <c r="P29" s="14" t="s">
         <v>53</v>
@@ -12542,14 +14053,14 @@
       <c r="Q29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="R29" s="18" t="s">
+      <c r="R29" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18" t="s">
+      <c r="S29" s="21"/>
+      <c r="T29" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="U29" s="18"/>
+      <c r="U29" s="21"/>
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
@@ -12558,24 +14069,24 @@
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
       <c r="H30" s="5"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
       <c r="O30" s="5"/>
       <c r="P30" s="13"/>
       <c r="Q30" s="4"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
@@ -12584,24 +14095,24 @@
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
       <c r="H31" s="5"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
       <c r="O31" s="5"/>
       <c r="P31" s="13"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
@@ -12617,17 +14128,17 @@
       <c r="H32" s="5"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
       <c r="O32" s="5"/>
       <c r="P32" s="13"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
@@ -12643,17 +14154,17 @@
       <c r="H33" s="5"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
       <c r="O33" s="5"/>
       <c r="P33" s="13"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
@@ -12685,31 +14196,31 @@
       <c r="X34" s="5"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="29" t="s">
+      <c r="I35" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="29"/>
-      <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
-      <c r="U35" s="29"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
       <c r="X35" s="5"/>
@@ -12718,46 +14229,46 @@
       <c r="A36" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18" t="s">
+      <c r="C36" s="21"/>
+      <c r="D36" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18" t="s">
+      <c r="E36" s="21"/>
+      <c r="F36" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G36" s="18"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="18" t="s">
+      <c r="I36" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="J36" s="18"/>
-      <c r="K36" s="22" t="s">
+      <c r="J36" s="21"/>
+      <c r="K36" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18" t="s">
+      <c r="L36" s="21"/>
+      <c r="M36" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18" t="s">
+      <c r="N36" s="21"/>
+      <c r="O36" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="P36" s="18"/>
+      <c r="P36" s="21"/>
       <c r="Q36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="R36" s="18" t="s">
+      <c r="R36" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="S36" s="18"/>
-      <c r="T36" s="18" t="s">
+      <c r="S36" s="21"/>
+      <c r="T36" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="U36" s="18"/>
+      <c r="U36" s="21"/>
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
       <c r="X36" s="5"/>
@@ -12766,176 +14277,176 @@
       <c r="A37" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18" t="s">
+      <c r="C37" s="21"/>
+      <c r="D37" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18" t="s">
+      <c r="E37" s="21"/>
+      <c r="F37" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="G37" s="18"/>
+      <c r="G37" s="21"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="30" t="s">
+      <c r="I37" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="J37" s="31"/>
-      <c r="K37" s="22" t="s">
+      <c r="J37" s="23"/>
+      <c r="K37" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18" t="s">
+      <c r="L37" s="21"/>
+      <c r="M37" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18" t="s">
+      <c r="N37" s="21"/>
+      <c r="O37" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="P37" s="18"/>
+      <c r="P37" s="21"/>
       <c r="Q37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="R37" s="18" t="s">
+      <c r="R37" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18" t="s">
+      <c r="S37" s="21"/>
+      <c r="T37" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="U37" s="18"/>
+      <c r="U37" s="21"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
     </row>
     <row r="38" spans="1:24">
       <c r="A38" s="16"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
       <c r="H38" s="5"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="33"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="25"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
       <c r="Q38" s="4"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18" t="s">
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="U38" s="18"/>
+      <c r="U38" s="21"/>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
       <c r="X38" s="5"/>
     </row>
     <row r="39" spans="1:24">
       <c r="A39" s="16"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
       <c r="H39" s="5"/>
       <c r="I39" s="17"/>
       <c r="J39" s="17"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
       <c r="Q39" s="4"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="16"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
       <c r="H40" s="5"/>
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
       <c r="Q40" s="4"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
     </row>
     <row r="41" spans="1:24">
       <c r="A41" s="16"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
       <c r="H41" s="5"/>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
     </row>
     <row r="42" spans="1:24">
       <c r="A42" s="16"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
       <c r="H42" s="5"/>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
       <c r="Q42" s="4"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
@@ -12994,6 +14505,238 @@
     </row>
   </sheetData>
   <mergeCells count="256">
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="T39:U39"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="T37:U37"/>
     <mergeCell ref="I10:W10"/>
     <mergeCell ref="I35:U35"/>
     <mergeCell ref="A35:G35"/>
@@ -13018,238 +14761,6 @@
     <mergeCell ref="O38:P38"/>
     <mergeCell ref="R38:S38"/>
     <mergeCell ref="T38:U38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="T39:U39"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13258,19 +14769,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4194BB0-32F4-4886-B67D-98C7D935108E}">
-  <dimension ref="A1"/>
+  <dimension ref="S20:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+    <sheetView tabSelected="1" topLeftCell="G58" workbookViewId="0">
+      <selection activeCell="Q87" sqref="Q87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="20" spans="19:20">
+      <c r="S20" t="s">
+        <v>76</v>
+      </c>
+      <c r="T20" s="18"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13323,7 +14842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81982883-1BDE-4282-B2B9-33F2A9AD9B5C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -13338,7 +14857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE28ACF3-421C-469B-9F62-03CCC065B3D1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="Z47" sqref="Z47"/>
     </sheetView>
   </sheetViews>

</xml_diff>